<commit_message>
(minor) PEP 8 issues.
</commit_message>
<xml_diff>
--- a/Analysis/Day 14 - Regolith Reservoir.xlsx
+++ b/Analysis/Day 14 - Regolith Reservoir.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PWeemaes\Documents\Miscellaneous\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PWeemaes\Python Projects\AoC2022\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495D7F5D-810C-44A4-97BA-6060B91058FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A68994-46AF-4652-A959-60B23A6BB391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9BD4E827-56F0-478D-9912-B3791E0B7C40}"/>
   </bookViews>
@@ -192,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -243,9 +243,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -264,10 +261,10 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -586,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D8083F-2B46-4AE5-86CA-AB01F187A48E}">
   <dimension ref="A1:BG118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="95" workbookViewId="0">
-      <selection activeCell="AL9" sqref="AL9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="95" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15:S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.5546875" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1597,51 +1594,51 @@
       <c r="AO16"/>
       <c r="AP16"/>
     </row>
-    <row r="17" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="21">
+    <row r="17" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="20">
         <f>E17-1</f>
         <v>0</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="20">
         <v>1</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="20">
         <f>E17+1</f>
         <v>2</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="20">
         <f t="shared" ref="G17:O17" si="2">F17+1</f>
         <v>3</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="20">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="20">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J17" s="20">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="K17" s="21">
+      <c r="K17" s="20">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="L17" s="21">
+      <c r="L17" s="20">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="M17" s="21">
+      <c r="M17" s="20">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="N17" s="21">
+      <c r="N17" s="20">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="O17" s="21">
+      <c r="O17" s="20">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
@@ -1661,8 +1658,8 @@
       <c r="AA17" s="25"/>
       <c r="AB17" s="25"/>
     </row>
-    <row r="18" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="23"/>
+    <row r="18" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="22"/>
       <c r="E18" s="2">
         <v>93</v>
       </c>
@@ -1690,10 +1687,10 @@
       <c r="M18" s="17">
         <v>1</v>
       </c>
-      <c r="O18" s="21"/>
-    </row>
-    <row r="19" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="23"/>
+      <c r="O18" s="20"/>
+    </row>
+    <row r="19" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="22"/>
       <c r="E19" s="2">
         <v>93</v>
       </c>
@@ -1721,10 +1718,10 @@
       <c r="M19" s="17">
         <v>2</v>
       </c>
-      <c r="O19" s="21"/>
-    </row>
-    <row r="20" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="23"/>
+      <c r="O19" s="20"/>
+    </row>
+    <row r="20" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="22"/>
       <c r="E20" s="2">
         <v>93</v>
       </c>
@@ -1752,10 +1749,10 @@
       <c r="M20" s="17">
         <v>3</v>
       </c>
-      <c r="O20" s="21"/>
-    </row>
-    <row r="21" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="23"/>
+      <c r="O20" s="20"/>
+    </row>
+    <row r="21" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="22"/>
       <c r="E21" s="2">
         <v>93</v>
       </c>
@@ -1780,10 +1777,10 @@
       <c r="L21" s="17">
         <v>4</v>
       </c>
-      <c r="O21" s="21"/>
-    </row>
-    <row r="22" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="23"/>
+      <c r="O21" s="20"/>
+    </row>
+    <row r="22" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="22"/>
       <c r="E22" s="2">
         <v>93</v>
       </c>
@@ -1811,10 +1808,10 @@
       <c r="M22" s="17">
         <v>5</v>
       </c>
-      <c r="O22" s="21"/>
-    </row>
-    <row r="23" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="23"/>
+      <c r="O22" s="20"/>
+    </row>
+    <row r="23" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="22"/>
       <c r="E23" s="2">
         <v>93</v>
       </c>
@@ -1839,10 +1836,10 @@
       <c r="L23" s="17">
         <v>6</v>
       </c>
-      <c r="O23" s="21"/>
-    </row>
-    <row r="24" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="23"/>
+      <c r="O23" s="20"/>
+    </row>
+    <row r="24" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="22"/>
       <c r="E24" s="2">
         <v>93</v>
       </c>
@@ -1867,10 +1864,10 @@
       <c r="L24" s="17">
         <v>7</v>
       </c>
-      <c r="O24" s="21"/>
-    </row>
-    <row r="25" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="23"/>
+      <c r="O24" s="20"/>
+    </row>
+    <row r="25" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="22"/>
       <c r="E25" s="2">
         <v>93</v>
       </c>
@@ -1892,10 +1889,10 @@
       <c r="K25" s="17">
         <v>8</v>
       </c>
-      <c r="O25" s="21"/>
-    </row>
-    <row r="26" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="23"/>
+      <c r="O25" s="20"/>
+    </row>
+    <row r="26" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="22"/>
       <c r="E26" s="2">
         <v>93</v>
       </c>
@@ -1923,10 +1920,10 @@
       <c r="M26" s="17">
         <v>9</v>
       </c>
-      <c r="O26" s="21"/>
-    </row>
-    <row r="27" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="23"/>
+      <c r="O26" s="20"/>
+    </row>
+    <row r="27" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="22"/>
       <c r="E27" s="2">
         <v>93</v>
       </c>
@@ -1951,10 +1948,10 @@
       <c r="L27" s="17">
         <v>10</v>
       </c>
-      <c r="O27" s="21"/>
-    </row>
-    <row r="28" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="23"/>
+      <c r="O27" s="20"/>
+    </row>
+    <row r="28" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="22"/>
       <c r="E28" s="2">
         <v>93</v>
       </c>
@@ -1976,10 +1973,10 @@
       <c r="K28" s="17">
         <v>11</v>
       </c>
-      <c r="O28" s="21"/>
-    </row>
-    <row r="29" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="23"/>
+      <c r="O28" s="20"/>
+    </row>
+    <row r="29" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="22"/>
       <c r="E29" s="2">
         <v>93</v>
       </c>
@@ -2001,34 +1998,10 @@
       <c r="K29" s="17">
         <v>12</v>
       </c>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="18"/>
-      <c r="T29" s="18"/>
-      <c r="U29" s="18"/>
-      <c r="V29" s="18"/>
-      <c r="W29" s="18"/>
-      <c r="X29" s="18"/>
-      <c r="Y29" s="18"/>
-      <c r="Z29" s="18"/>
-      <c r="AA29" s="18"/>
-      <c r="AB29" s="18"/>
-      <c r="AC29" s="18"/>
-      <c r="AD29" s="18"/>
-      <c r="AE29" s="18"/>
-      <c r="AF29" s="18"/>
-      <c r="AG29" s="18"/>
-      <c r="AH29" s="18"/>
-      <c r="AI29" s="18"/>
-      <c r="AJ29" s="18"/>
-    </row>
-    <row r="30" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="23"/>
+      <c r="O29" s="20"/>
+    </row>
+    <row r="30" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="22"/>
       <c r="E30" s="2">
         <v>93</v>
       </c>
@@ -2048,10 +2021,10 @@
         <v>13</v>
       </c>
       <c r="K30" s="17"/>
-      <c r="O30" s="21"/>
-    </row>
-    <row r="31" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="23"/>
+      <c r="O30" s="20"/>
+    </row>
+    <row r="31" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="22"/>
       <c r="E31" s="2">
         <v>93</v>
       </c>
@@ -2070,10 +2043,10 @@
       <c r="J31" s="17">
         <v>14</v>
       </c>
-      <c r="O31" s="21"/>
-    </row>
-    <row r="32" spans="4:36" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="23"/>
+      <c r="O31" s="20"/>
+    </row>
+    <row r="32" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="22"/>
       <c r="E32" s="2">
         <v>93</v>
       </c>
@@ -2092,10 +2065,10 @@
       <c r="J32" s="17">
         <v>15</v>
       </c>
-      <c r="O32" s="21"/>
+      <c r="O32" s="20"/>
     </row>
     <row r="33" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="23"/>
+      <c r="D33" s="22"/>
       <c r="E33" s="2">
         <v>93</v>
       </c>
@@ -2112,10 +2085,10 @@
         <v>16</v>
       </c>
       <c r="J33" s="17"/>
-      <c r="O33" s="21"/>
+      <c r="O33" s="20"/>
     </row>
     <row r="34" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="23"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="2">
         <v>93</v>
       </c>
@@ -2131,10 +2104,10 @@
       <c r="I34" s="17">
         <v>17</v>
       </c>
-      <c r="O34" s="21"/>
+      <c r="O34" s="20"/>
     </row>
     <row r="35" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="23"/>
+      <c r="D35" s="22"/>
       <c r="E35" s="2">
         <v>93</v>
       </c>
@@ -2150,10 +2123,10 @@
       <c r="I35" s="17">
         <v>18</v>
       </c>
-      <c r="O35" s="21"/>
+      <c r="O35" s="20"/>
     </row>
     <row r="36" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="23"/>
+      <c r="D36" s="22"/>
       <c r="E36" s="2">
         <v>93</v>
       </c>
@@ -2166,10 +2139,10 @@
       <c r="H36" s="17">
         <v>19</v>
       </c>
-      <c r="O36" s="21"/>
+      <c r="O36" s="20"/>
     </row>
     <row r="37" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="23"/>
+      <c r="D37" s="22"/>
       <c r="E37" s="2">
         <v>93</v>
       </c>
@@ -2182,10 +2155,10 @@
       <c r="H37" s="17">
         <v>20</v>
       </c>
-      <c r="O37" s="21"/>
+      <c r="O37" s="20"/>
     </row>
     <row r="38" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="23"/>
+      <c r="D38" s="22"/>
       <c r="E38" s="2">
         <v>93</v>
       </c>
@@ -2198,10 +2171,10 @@
       <c r="H38" s="17">
         <v>21</v>
       </c>
-      <c r="O38" s="21"/>
+      <c r="O38" s="20"/>
     </row>
     <row r="39" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D39" s="23"/>
+      <c r="D39" s="22"/>
       <c r="E39" s="2">
         <v>93</v>
       </c>
@@ -2211,10 +2184,10 @@
       <c r="G39" s="17">
         <v>22</v>
       </c>
-      <c r="O39" s="21"/>
+      <c r="O39" s="20"/>
     </row>
     <row r="40" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="23"/>
+      <c r="D40" s="22"/>
       <c r="E40" s="2">
         <v>93</v>
       </c>
@@ -2233,10 +2206,10 @@
       <c r="J40" s="17">
         <v>23</v>
       </c>
-      <c r="O40" s="21"/>
+      <c r="O40" s="20"/>
     </row>
     <row r="41" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="23"/>
+      <c r="D41" s="22"/>
       <c r="E41" s="2">
         <v>93</v>
       </c>
@@ -2249,76 +2222,76 @@
       <c r="H41" s="2">
         <v>40</v>
       </c>
-      <c r="I41" s="19">
+      <c r="I41" s="18">
         <v>39</v>
       </c>
-      <c r="J41" s="19">
+      <c r="J41" s="18">
         <v>38</v>
       </c>
-      <c r="K41" s="19">
+      <c r="K41" s="18">
         <v>37</v>
       </c>
-      <c r="L41" s="20">
+      <c r="L41" s="19">
         <v>31</v>
       </c>
       <c r="M41" s="17">
         <v>24</v>
       </c>
-      <c r="O41" s="21"/>
+      <c r="O41" s="20"/>
     </row>
     <row r="42" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="23"/>
-      <c r="E42" s="23">
-        <v>93</v>
-      </c>
-      <c r="F42" s="23">
-        <v>44</v>
-      </c>
-      <c r="G42" s="23">
+      <c r="D42" s="22"/>
+      <c r="E42" s="22">
+        <v>93</v>
+      </c>
+      <c r="F42" s="22">
+        <v>44</v>
+      </c>
+      <c r="G42" s="22">
         <v>41</v>
       </c>
-      <c r="H42" s="23">
+      <c r="H42" s="22">
         <v>40</v>
       </c>
-      <c r="I42" s="24">
+      <c r="I42" s="23">
         <v>39</v>
       </c>
-      <c r="J42" s="24">
+      <c r="J42" s="23">
         <v>38</v>
       </c>
-      <c r="K42" s="24">
+      <c r="K42" s="23">
         <v>37</v>
       </c>
-      <c r="L42" s="24">
+      <c r="L42" s="23">
         <v>31</v>
       </c>
-      <c r="M42" s="23">
+      <c r="M42" s="22">
         <v>29</v>
       </c>
-      <c r="N42" s="21">
+      <c r="N42" s="20">
         <v>28</v>
       </c>
-      <c r="O42" s="22">
+      <c r="O42" s="21">
         <v>25</v>
       </c>
-      <c r="P42" s="26" t="s">
+      <c r="P42" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="Q42" s="26"/>
-      <c r="R42" s="26"/>
-      <c r="S42" s="26"/>
-      <c r="T42" s="26"/>
-      <c r="U42" s="26"/>
-      <c r="V42" s="26"/>
-      <c r="W42" s="26"/>
-      <c r="X42" s="26"/>
-      <c r="Y42" s="26"/>
-      <c r="Z42" s="26"/>
-      <c r="AA42" s="26"/>
-      <c r="AB42" s="26"/>
+      <c r="Q42" s="24"/>
+      <c r="R42" s="24"/>
+      <c r="S42" s="24"/>
+      <c r="T42" s="24"/>
+      <c r="U42" s="24"/>
+      <c r="V42" s="24"/>
+      <c r="W42" s="24"/>
+      <c r="X42" s="24"/>
+      <c r="Y42" s="24"/>
+      <c r="Z42" s="24"/>
+      <c r="AA42" s="24"/>
+      <c r="AB42" s="24"/>
     </row>
     <row r="43" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="23"/>
+      <c r="D43" s="22"/>
       <c r="E43" s="2">
         <v>93</v>
       </c>
@@ -2331,16 +2304,16 @@
       <c r="H43" s="2">
         <v>40</v>
       </c>
-      <c r="I43" s="19">
+      <c r="I43" s="18">
         <v>39</v>
       </c>
-      <c r="J43" s="19">
+      <c r="J43" s="18">
         <v>38</v>
       </c>
-      <c r="K43" s="19">
+      <c r="K43" s="18">
         <v>37</v>
       </c>
-      <c r="L43" s="19">
+      <c r="L43" s="18">
         <v>31</v>
       </c>
       <c r="M43" s="2">
@@ -2349,12 +2322,12 @@
       <c r="N43" s="4">
         <v>28</v>
       </c>
-      <c r="O43" s="22">
+      <c r="O43" s="21">
         <v>26</v>
       </c>
     </row>
     <row r="44" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="23"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="2">
         <v>93</v>
       </c>
@@ -2367,16 +2340,16 @@
       <c r="H44" s="2">
         <v>40</v>
       </c>
-      <c r="I44" s="19">
+      <c r="I44" s="18">
         <v>39</v>
       </c>
-      <c r="J44" s="19">
+      <c r="J44" s="18">
         <v>38</v>
       </c>
-      <c r="K44" s="19">
+      <c r="K44" s="18">
         <v>37</v>
       </c>
-      <c r="L44" s="19">
+      <c r="L44" s="18">
         <v>31</v>
       </c>
       <c r="M44" s="2">
@@ -2385,12 +2358,12 @@
       <c r="N44" s="4">
         <v>28</v>
       </c>
-      <c r="O44" s="22">
+      <c r="O44" s="21">
         <v>27</v>
       </c>
     </row>
     <row r="45" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="23"/>
+      <c r="D45" s="22"/>
       <c r="E45" s="2">
         <v>93</v>
       </c>
@@ -2403,16 +2376,16 @@
       <c r="H45" s="2">
         <v>40</v>
       </c>
-      <c r="I45" s="19">
+      <c r="I45" s="18">
         <v>39</v>
       </c>
-      <c r="J45" s="19">
+      <c r="J45" s="18">
         <v>38</v>
       </c>
-      <c r="K45" s="19">
+      <c r="K45" s="18">
         <v>37</v>
       </c>
-      <c r="L45" s="19">
+      <c r="L45" s="18">
         <v>31</v>
       </c>
       <c r="M45" s="4">
@@ -2421,10 +2394,10 @@
       <c r="N45" s="17">
         <v>28</v>
       </c>
-      <c r="O45" s="21"/>
+      <c r="O45" s="20"/>
     </row>
     <row r="46" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="23"/>
+      <c r="D46" s="22"/>
       <c r="E46" s="2">
         <v>93</v>
       </c>
@@ -2437,25 +2410,25 @@
       <c r="H46" s="2">
         <v>40</v>
       </c>
-      <c r="I46" s="19">
+      <c r="I46" s="18">
         <v>39</v>
       </c>
-      <c r="J46" s="19">
+      <c r="J46" s="18">
         <v>38</v>
       </c>
-      <c r="K46" s="19">
+      <c r="K46" s="18">
         <v>37</v>
       </c>
-      <c r="L46" s="19">
+      <c r="L46" s="18">
         <v>31</v>
       </c>
       <c r="M46" s="17">
         <v>29</v>
       </c>
-      <c r="O46" s="21"/>
+      <c r="O46" s="20"/>
     </row>
     <row r="47" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="23"/>
+      <c r="D47" s="22"/>
       <c r="E47" s="2">
         <v>93</v>
       </c>
@@ -2468,25 +2441,25 @@
       <c r="H47" s="2">
         <v>40</v>
       </c>
-      <c r="I47" s="19">
+      <c r="I47" s="18">
         <v>39</v>
       </c>
-      <c r="J47" s="19">
+      <c r="J47" s="18">
         <v>38</v>
       </c>
-      <c r="K47" s="19">
+      <c r="K47" s="18">
         <v>37</v>
       </c>
-      <c r="L47" s="19">
+      <c r="L47" s="18">
         <v>31</v>
       </c>
       <c r="M47" s="17">
         <v>30</v>
       </c>
-      <c r="O47" s="21"/>
+      <c r="O47" s="20"/>
     </row>
     <row r="48" spans="4:28" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="23"/>
+      <c r="D48" s="22"/>
       <c r="E48" s="2">
         <v>93</v>
       </c>
@@ -2499,22 +2472,22 @@
       <c r="H48" s="2">
         <v>40</v>
       </c>
-      <c r="I48" s="19">
+      <c r="I48" s="18">
         <v>39</v>
       </c>
-      <c r="J48" s="19">
+      <c r="J48" s="18">
         <v>38</v>
       </c>
-      <c r="K48" s="19">
+      <c r="K48" s="18">
         <v>37</v>
       </c>
       <c r="L48" s="17">
         <v>31</v>
       </c>
-      <c r="O48" s="21"/>
+      <c r="O48" s="20"/>
     </row>
     <row r="49" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="23"/>
+      <c r="D49" s="22"/>
       <c r="E49" s="2">
         <v>93</v>
       </c>
@@ -2527,13 +2500,13 @@
       <c r="H49" s="2">
         <v>40</v>
       </c>
-      <c r="I49" s="19">
+      <c r="I49" s="18">
         <v>39</v>
       </c>
-      <c r="J49" s="19">
+      <c r="J49" s="18">
         <v>38</v>
       </c>
-      <c r="K49" s="19">
+      <c r="K49" s="18">
         <v>37</v>
       </c>
       <c r="L49" s="2">
@@ -2545,12 +2518,12 @@
       <c r="N49" s="2">
         <v>33</v>
       </c>
-      <c r="O49" s="22">
+      <c r="O49" s="21">
         <v>32</v>
       </c>
     </row>
     <row r="50" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D50" s="23"/>
+      <c r="D50" s="22"/>
       <c r="E50" s="2">
         <v>93</v>
       </c>
@@ -2563,13 +2536,13 @@
       <c r="H50" s="2">
         <v>40</v>
       </c>
-      <c r="I50" s="19">
+      <c r="I50" s="18">
         <v>39</v>
       </c>
-      <c r="J50" s="19">
+      <c r="J50" s="18">
         <v>38</v>
       </c>
-      <c r="K50" s="19">
+      <c r="K50" s="18">
         <v>37</v>
       </c>
       <c r="L50" s="2">
@@ -2581,10 +2554,10 @@
       <c r="N50" s="17">
         <v>33</v>
       </c>
-      <c r="O50" s="21"/>
+      <c r="O50" s="20"/>
     </row>
     <row r="51" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="23"/>
+      <c r="D51" s="22"/>
       <c r="E51" s="2">
         <v>93</v>
       </c>
@@ -2597,13 +2570,13 @@
       <c r="H51" s="2">
         <v>40</v>
       </c>
-      <c r="I51" s="19">
+      <c r="I51" s="18">
         <v>39</v>
       </c>
-      <c r="J51" s="19">
+      <c r="J51" s="18">
         <v>38</v>
       </c>
-      <c r="K51" s="19">
+      <c r="K51" s="18">
         <v>37</v>
       </c>
       <c r="L51" s="2">
@@ -2612,10 +2585,10 @@
       <c r="M51" s="17">
         <v>34</v>
       </c>
-      <c r="O51" s="21"/>
+      <c r="O51" s="20"/>
     </row>
     <row r="52" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="23"/>
+      <c r="D52" s="22"/>
       <c r="E52" s="2">
         <v>93</v>
       </c>
@@ -2628,22 +2601,22 @@
       <c r="H52" s="2">
         <v>40</v>
       </c>
-      <c r="I52" s="19">
+      <c r="I52" s="18">
         <v>39</v>
       </c>
-      <c r="J52" s="19">
+      <c r="J52" s="18">
         <v>38</v>
       </c>
-      <c r="K52" s="19">
+      <c r="K52" s="18">
         <v>37</v>
       </c>
       <c r="L52" s="17">
         <v>35</v>
       </c>
-      <c r="O52" s="21"/>
+      <c r="O52" s="20"/>
     </row>
     <row r="53" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="23"/>
+      <c r="D53" s="22"/>
       <c r="E53" s="2">
         <v>93</v>
       </c>
@@ -2656,22 +2629,22 @@
       <c r="H53" s="2">
         <v>40</v>
       </c>
-      <c r="I53" s="19">
+      <c r="I53" s="18">
         <v>39</v>
       </c>
-      <c r="J53" s="19">
+      <c r="J53" s="18">
         <v>38</v>
       </c>
-      <c r="K53" s="19">
+      <c r="K53" s="18">
         <v>37</v>
       </c>
       <c r="L53" s="17">
         <v>36</v>
       </c>
-      <c r="O53" s="21"/>
+      <c r="O53" s="20"/>
     </row>
     <row r="54" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="23"/>
+      <c r="D54" s="22"/>
       <c r="E54" s="2">
         <v>93</v>
       </c>
@@ -2684,19 +2657,19 @@
       <c r="H54" s="2">
         <v>40</v>
       </c>
-      <c r="I54" s="19">
+      <c r="I54" s="18">
         <v>39</v>
       </c>
-      <c r="J54" s="19">
+      <c r="J54" s="18">
         <v>38</v>
       </c>
       <c r="K54" s="17">
         <v>37</v>
       </c>
-      <c r="O54" s="21"/>
+      <c r="O54" s="20"/>
     </row>
     <row r="55" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="23"/>
+      <c r="D55" s="22"/>
       <c r="E55" s="2">
         <v>93</v>
       </c>
@@ -2709,16 +2682,16 @@
       <c r="H55" s="2">
         <v>40</v>
       </c>
-      <c r="I55" s="19">
+      <c r="I55" s="18">
         <v>39</v>
       </c>
       <c r="J55" s="17">
         <v>38</v>
       </c>
-      <c r="O55" s="21"/>
+      <c r="O55" s="20"/>
     </row>
     <row r="56" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="23"/>
+      <c r="D56" s="22"/>
       <c r="E56" s="2">
         <v>93</v>
       </c>
@@ -2734,11 +2707,11 @@
       <c r="I56" s="17">
         <v>39</v>
       </c>
-      <c r="J56" s="19"/>
-      <c r="O56" s="21"/>
+      <c r="J56" s="18"/>
+      <c r="O56" s="20"/>
     </row>
     <row r="57" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D57" s="23"/>
+      <c r="D57" s="22"/>
       <c r="E57" s="2">
         <v>93</v>
       </c>
@@ -2751,12 +2724,12 @@
       <c r="H57" s="17">
         <v>40</v>
       </c>
-      <c r="I57" s="19"/>
-      <c r="J57" s="19"/>
-      <c r="O57" s="21"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
+      <c r="O57" s="20"/>
     </row>
     <row r="58" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D58" s="23"/>
+      <c r="D58" s="22"/>
       <c r="E58" s="2">
         <v>93</v>
       </c>
@@ -2766,12 +2739,12 @@
       <c r="G58" s="17">
         <v>41</v>
       </c>
-      <c r="I58" s="19"/>
-      <c r="J58" s="19"/>
-      <c r="O58" s="21"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="O58" s="20"/>
     </row>
     <row r="59" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="23"/>
+      <c r="D59" s="22"/>
       <c r="E59" s="2">
         <v>93</v>
       </c>
@@ -2784,10 +2757,10 @@
       <c r="H59" s="17">
         <v>42</v>
       </c>
-      <c r="O59" s="21"/>
+      <c r="O59" s="20"/>
     </row>
     <row r="60" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="23"/>
+      <c r="D60" s="22"/>
       <c r="E60" s="2">
         <v>93</v>
       </c>
@@ -2797,20 +2770,20 @@
       <c r="G60" s="17">
         <v>43</v>
       </c>
-      <c r="O60" s="21"/>
+      <c r="O60" s="20"/>
     </row>
     <row r="61" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D61" s="23"/>
+      <c r="D61" s="22"/>
       <c r="E61" s="2">
         <v>93</v>
       </c>
       <c r="F61" s="17">
         <v>44</v>
       </c>
-      <c r="O61" s="21"/>
+      <c r="O61" s="20"/>
     </row>
     <row r="62" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D62" s="23"/>
+      <c r="D62" s="22"/>
       <c r="E62" s="2">
         <v>93</v>
       </c>
@@ -2841,12 +2814,12 @@
       <c r="N62" s="2">
         <v>46</v>
       </c>
-      <c r="O62" s="22">
+      <c r="O62" s="21">
         <v>45</v>
       </c>
     </row>
     <row r="63" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="23"/>
+      <c r="D63" s="22"/>
       <c r="E63" s="2">
         <v>93</v>
       </c>
@@ -2877,10 +2850,10 @@
       <c r="N63" s="17">
         <v>46</v>
       </c>
-      <c r="O63" s="21"/>
+      <c r="O63" s="20"/>
     </row>
     <row r="64" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="23"/>
+      <c r="D64" s="22"/>
       <c r="E64" s="2">
         <v>93</v>
       </c>
@@ -2908,10 +2881,10 @@
       <c r="M64" s="17">
         <v>47</v>
       </c>
-      <c r="O64" s="21"/>
+      <c r="O64" s="20"/>
     </row>
     <row r="65" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="23"/>
+      <c r="D65" s="22"/>
       <c r="E65" s="2">
         <v>93</v>
       </c>
@@ -2936,10 +2909,10 @@
       <c r="L65" s="17">
         <v>48</v>
       </c>
-      <c r="O65" s="21"/>
+      <c r="O65" s="20"/>
     </row>
     <row r="66" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="23"/>
+      <c r="D66" s="22"/>
       <c r="E66" s="2">
         <v>93</v>
       </c>
@@ -2961,10 +2934,10 @@
       <c r="K66" s="17">
         <v>49</v>
       </c>
-      <c r="O66" s="21"/>
+      <c r="O66" s="20"/>
     </row>
     <row r="67" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D67" s="23"/>
+      <c r="D67" s="22"/>
       <c r="E67" s="2">
         <v>93</v>
       </c>
@@ -2983,10 +2956,10 @@
       <c r="J67" s="17">
         <v>50</v>
       </c>
-      <c r="O67" s="21"/>
+      <c r="O67" s="20"/>
     </row>
     <row r="68" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D68" s="23"/>
+      <c r="D68" s="22"/>
       <c r="E68" s="2">
         <v>93</v>
       </c>
@@ -3002,10 +2975,10 @@
       <c r="I68" s="17">
         <v>51</v>
       </c>
-      <c r="O68" s="21"/>
+      <c r="O68" s="20"/>
     </row>
     <row r="69" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D69" s="23"/>
+      <c r="D69" s="22"/>
       <c r="E69" s="2">
         <v>93</v>
       </c>
@@ -3018,10 +2991,10 @@
       <c r="H69" s="17">
         <v>52</v>
       </c>
-      <c r="O69" s="21"/>
+      <c r="O69" s="20"/>
     </row>
     <row r="70" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="23"/>
+      <c r="D70" s="22"/>
       <c r="E70" s="2">
         <v>93</v>
       </c>
@@ -3031,20 +3004,20 @@
       <c r="G70" s="17">
         <v>53</v>
       </c>
-      <c r="O70" s="21"/>
+      <c r="O70" s="20"/>
     </row>
     <row r="71" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="23"/>
+      <c r="D71" s="22"/>
       <c r="E71" s="2">
         <v>93</v>
       </c>
       <c r="F71" s="17">
         <v>54</v>
       </c>
-      <c r="O71" s="21"/>
+      <c r="O71" s="20"/>
     </row>
     <row r="72" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D72" s="23"/>
+      <c r="D72" s="22"/>
       <c r="E72" s="2">
         <v>93</v>
       </c>
@@ -3075,13 +3048,13 @@
       <c r="N72" s="2">
         <v>58</v>
       </c>
-      <c r="O72" s="22">
+      <c r="O72" s="21">
         <v>55</v>
       </c>
       <c r="V72"/>
     </row>
     <row r="73" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D73" s="23"/>
+      <c r="D73" s="22"/>
       <c r="E73" s="2">
         <v>93</v>
       </c>
@@ -3112,13 +3085,13 @@
       <c r="N73" s="2">
         <v>58</v>
       </c>
-      <c r="O73" s="22">
+      <c r="O73" s="21">
         <v>56</v>
       </c>
       <c r="V73"/>
     </row>
     <row r="74" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D74" s="23"/>
+      <c r="D74" s="22"/>
       <c r="E74" s="2">
         <v>93</v>
       </c>
@@ -3149,13 +3122,13 @@
       <c r="N74" s="2">
         <v>58</v>
       </c>
-      <c r="O74" s="22">
+      <c r="O74" s="21">
         <v>57</v>
       </c>
       <c r="V74"/>
     </row>
     <row r="75" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D75" s="23"/>
+      <c r="D75" s="22"/>
       <c r="E75" s="2">
         <v>93</v>
       </c>
@@ -3186,11 +3159,11 @@
       <c r="N75" s="17">
         <v>58</v>
       </c>
-      <c r="O75" s="21"/>
+      <c r="O75" s="20"/>
       <c r="V75"/>
     </row>
     <row r="76" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D76" s="23"/>
+      <c r="D76" s="22"/>
       <c r="E76" s="2">
         <v>93</v>
       </c>
@@ -3221,13 +3194,13 @@
       <c r="N76" s="2">
         <v>60</v>
       </c>
-      <c r="O76" s="22">
+      <c r="O76" s="21">
         <v>59</v>
       </c>
       <c r="V76"/>
     </row>
     <row r="77" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D77" s="23"/>
+      <c r="D77" s="22"/>
       <c r="E77" s="2">
         <v>93</v>
       </c>
@@ -3258,11 +3231,11 @@
       <c r="N77" s="17">
         <v>60</v>
       </c>
-      <c r="O77" s="22"/>
+      <c r="O77" s="21"/>
       <c r="V77"/>
     </row>
     <row r="78" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D78" s="23"/>
+      <c r="D78" s="22"/>
       <c r="E78" s="2">
         <v>93</v>
       </c>
@@ -3293,13 +3266,13 @@
       <c r="N78" s="2">
         <v>62</v>
       </c>
-      <c r="O78" s="22">
+      <c r="O78" s="21">
         <v>61</v>
       </c>
       <c r="V78"/>
     </row>
     <row r="79" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D79" s="23"/>
+      <c r="D79" s="22"/>
       <c r="E79" s="2">
         <v>93</v>
       </c>
@@ -3330,10 +3303,10 @@
       <c r="N79" s="17">
         <v>62</v>
       </c>
-      <c r="O79" s="22"/>
+      <c r="O79" s="21"/>
     </row>
     <row r="80" spans="4:22" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D80" s="23"/>
+      <c r="D80" s="22"/>
       <c r="E80" s="2">
         <v>93</v>
       </c>
@@ -3361,10 +3334,10 @@
       <c r="M80" s="17">
         <v>63</v>
       </c>
-      <c r="O80" s="22"/>
+      <c r="O80" s="21"/>
     </row>
     <row r="81" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D81" s="23"/>
+      <c r="D81" s="22"/>
       <c r="E81" s="2">
         <v>93</v>
       </c>
@@ -3392,10 +3365,10 @@
       <c r="M81" s="17">
         <v>64</v>
       </c>
-      <c r="O81" s="22"/>
+      <c r="O81" s="21"/>
     </row>
     <row r="82" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D82" s="23"/>
+      <c r="D82" s="22"/>
       <c r="E82" s="2">
         <v>93</v>
       </c>
@@ -3426,12 +3399,12 @@
       <c r="N82" s="2">
         <v>66</v>
       </c>
-      <c r="O82" s="22">
+      <c r="O82" s="21">
         <v>65</v>
       </c>
     </row>
     <row r="83" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D83" s="23"/>
+      <c r="D83" s="22"/>
       <c r="E83" s="2">
         <v>93</v>
       </c>
@@ -3462,10 +3435,10 @@
       <c r="N83" s="17">
         <v>66</v>
       </c>
-      <c r="O83" s="22"/>
+      <c r="O83" s="21"/>
     </row>
     <row r="84" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D84" s="23"/>
+      <c r="D84" s="22"/>
       <c r="E84" s="2">
         <v>93</v>
       </c>
@@ -3493,10 +3466,10 @@
       <c r="M84" s="17">
         <v>67</v>
       </c>
-      <c r="O84" s="22"/>
+      <c r="O84" s="21"/>
     </row>
     <row r="85" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D85" s="23"/>
+      <c r="D85" s="22"/>
       <c r="E85" s="2">
         <v>93</v>
       </c>
@@ -3521,10 +3494,10 @@
       <c r="L85" s="17">
         <v>68</v>
       </c>
-      <c r="O85" s="22"/>
+      <c r="O85" s="21"/>
     </row>
     <row r="86" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D86" s="23"/>
+      <c r="D86" s="22"/>
       <c r="E86" s="2">
         <v>93</v>
       </c>
@@ -3549,10 +3522,10 @@
       <c r="L86" s="17">
         <v>69</v>
       </c>
-      <c r="O86" s="22"/>
+      <c r="O86" s="21"/>
     </row>
     <row r="87" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D87" s="23"/>
+      <c r="D87" s="22"/>
       <c r="E87" s="2">
         <v>93</v>
       </c>
@@ -3583,12 +3556,12 @@
       <c r="N87" s="2">
         <v>71</v>
       </c>
-      <c r="O87" s="22">
+      <c r="O87" s="21">
         <v>70</v>
       </c>
     </row>
     <row r="88" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D88" s="23"/>
+      <c r="D88" s="22"/>
       <c r="E88" s="2">
         <v>93</v>
       </c>
@@ -3619,10 +3592,10 @@
       <c r="N88" s="17">
         <v>71</v>
       </c>
-      <c r="O88" s="22"/>
+      <c r="O88" s="21"/>
     </row>
     <row r="89" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D89" s="23"/>
+      <c r="D89" s="22"/>
       <c r="E89" s="2">
         <v>93</v>
       </c>
@@ -3650,10 +3623,10 @@
       <c r="M89" s="17">
         <v>72</v>
       </c>
-      <c r="O89" s="22"/>
+      <c r="O89" s="21"/>
     </row>
     <row r="90" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D90" s="23"/>
+      <c r="D90" s="22"/>
       <c r="E90" s="2">
         <v>93</v>
       </c>
@@ -3678,10 +3651,10 @@
       <c r="L90" s="17">
         <v>73</v>
       </c>
-      <c r="O90" s="22"/>
+      <c r="O90" s="21"/>
     </row>
     <row r="91" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D91" s="23"/>
+      <c r="D91" s="22"/>
       <c r="E91" s="2">
         <v>93</v>
       </c>
@@ -3703,10 +3676,10 @@
       <c r="K91" s="17">
         <v>74</v>
       </c>
-      <c r="O91" s="22"/>
+      <c r="O91" s="21"/>
     </row>
     <row r="92" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D92" s="23"/>
+      <c r="D92" s="22"/>
       <c r="E92" s="2">
         <v>93</v>
       </c>
@@ -3728,10 +3701,10 @@
       <c r="K92" s="17">
         <v>75</v>
       </c>
-      <c r="O92" s="22"/>
+      <c r="O92" s="21"/>
     </row>
     <row r="93" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D93" s="23"/>
+      <c r="D93" s="22"/>
       <c r="E93" s="2">
         <v>93</v>
       </c>
@@ -3762,12 +3735,12 @@
       <c r="N93" s="2">
         <v>77</v>
       </c>
-      <c r="O93" s="22">
+      <c r="O93" s="21">
         <v>76</v>
       </c>
     </row>
     <row r="94" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D94" s="23"/>
+      <c r="D94" s="22"/>
       <c r="E94" s="2">
         <v>93</v>
       </c>
@@ -3798,10 +3771,10 @@
       <c r="N94" s="17">
         <v>77</v>
       </c>
-      <c r="O94" s="22"/>
+      <c r="O94" s="21"/>
     </row>
     <row r="95" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D95" s="23"/>
+      <c r="D95" s="22"/>
       <c r="E95" s="2">
         <v>93</v>
       </c>
@@ -3829,10 +3802,10 @@
       <c r="M95" s="17">
         <v>78</v>
       </c>
-      <c r="O95" s="22"/>
+      <c r="O95" s="21"/>
     </row>
     <row r="96" spans="4:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D96" s="23"/>
+      <c r="D96" s="22"/>
       <c r="E96" s="2">
         <v>93</v>
       </c>
@@ -3857,10 +3830,10 @@
       <c r="L96" s="17">
         <v>79</v>
       </c>
-      <c r="O96" s="22"/>
+      <c r="O96" s="21"/>
     </row>
     <row r="97" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D97" s="23"/>
+      <c r="D97" s="22"/>
       <c r="E97" s="2">
         <v>93</v>
       </c>
@@ -3882,10 +3855,10 @@
       <c r="K97" s="17">
         <v>80</v>
       </c>
-      <c r="O97" s="22"/>
+      <c r="O97" s="21"/>
     </row>
     <row r="98" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D98" s="23"/>
+      <c r="D98" s="22"/>
       <c r="E98" s="2">
         <v>93</v>
       </c>
@@ -3904,10 +3877,10 @@
       <c r="J98" s="17">
         <v>81</v>
       </c>
-      <c r="O98" s="22"/>
+      <c r="O98" s="21"/>
     </row>
     <row r="99" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D99" s="23"/>
+      <c r="D99" s="22"/>
       <c r="E99" s="2">
         <v>93</v>
       </c>
@@ -3926,10 +3899,10 @@
       <c r="J99" s="17">
         <v>82</v>
       </c>
-      <c r="O99" s="22"/>
+      <c r="O99" s="21"/>
     </row>
     <row r="100" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D100" s="23"/>
+      <c r="D100" s="22"/>
       <c r="E100" s="2">
         <v>93</v>
       </c>
@@ -3960,12 +3933,12 @@
       <c r="N100" s="2">
         <v>84</v>
       </c>
-      <c r="O100" s="22">
+      <c r="O100" s="21">
         <v>83</v>
       </c>
     </row>
     <row r="101" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D101" s="23"/>
+      <c r="D101" s="22"/>
       <c r="E101" s="2">
         <v>93</v>
       </c>
@@ -3996,10 +3969,10 @@
       <c r="N101" s="17">
         <v>84</v>
       </c>
-      <c r="O101" s="22"/>
+      <c r="O101" s="21"/>
     </row>
     <row r="102" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D102" s="23"/>
+      <c r="D102" s="22"/>
       <c r="E102" s="2">
         <v>93</v>
       </c>
@@ -4027,10 +4000,10 @@
       <c r="M102" s="17">
         <v>85</v>
       </c>
-      <c r="O102" s="22"/>
+      <c r="O102" s="21"/>
     </row>
     <row r="103" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D103" s="23"/>
+      <c r="D103" s="22"/>
       <c r="E103" s="2">
         <v>93</v>
       </c>
@@ -4055,10 +4028,10 @@
       <c r="L103" s="17">
         <v>86</v>
       </c>
-      <c r="O103" s="22"/>
+      <c r="O103" s="21"/>
     </row>
     <row r="104" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D104" s="23"/>
+      <c r="D104" s="22"/>
       <c r="E104" s="2">
         <v>93</v>
       </c>
@@ -4080,10 +4053,10 @@
       <c r="K104" s="17">
         <v>87</v>
       </c>
-      <c r="O104" s="22"/>
+      <c r="O104" s="21"/>
     </row>
     <row r="105" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D105" s="23"/>
+      <c r="D105" s="22"/>
       <c r="E105" s="2">
         <v>93</v>
       </c>
@@ -4102,10 +4075,10 @@
       <c r="J105" s="17">
         <v>88</v>
       </c>
-      <c r="O105" s="22"/>
+      <c r="O105" s="21"/>
     </row>
     <row r="106" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D106" s="23"/>
+      <c r="D106" s="22"/>
       <c r="E106" s="2">
         <v>93</v>
       </c>
@@ -4121,10 +4094,10 @@
       <c r="I106" s="17">
         <v>89</v>
       </c>
-      <c r="O106" s="22"/>
+      <c r="O106" s="21"/>
     </row>
     <row r="107" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D107" s="23"/>
+      <c r="D107" s="22"/>
       <c r="E107" s="2">
         <v>93</v>
       </c>
@@ -4137,10 +4110,10 @@
       <c r="H107" s="17">
         <v>90</v>
       </c>
-      <c r="O107" s="22"/>
+      <c r="O107" s="21"/>
     </row>
     <row r="108" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D108" s="23"/>
+      <c r="D108" s="22"/>
       <c r="E108" s="2">
         <v>93</v>
       </c>
@@ -4150,57 +4123,57 @@
       <c r="G108" s="17">
         <v>91</v>
       </c>
-      <c r="O108" s="22"/>
+      <c r="O108" s="21"/>
     </row>
     <row r="109" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D109" s="23"/>
+      <c r="D109" s="22"/>
       <c r="E109" s="2">
         <v>93</v>
       </c>
       <c r="F109" s="17">
         <v>92</v>
       </c>
-      <c r="O109" s="22"/>
+      <c r="O109" s="21"/>
     </row>
     <row r="110" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D110" s="23"/>
+      <c r="D110" s="22"/>
       <c r="E110" s="17">
         <v>93</v>
       </c>
-      <c r="O110" s="22"/>
+      <c r="O110" s="21"/>
     </row>
     <row r="111" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D111" s="23"/>
-      <c r="E111" s="23"/>
-      <c r="F111" s="23"/>
-      <c r="G111" s="23"/>
-      <c r="H111" s="23"/>
-      <c r="I111" s="23"/>
-      <c r="J111" s="23"/>
-      <c r="K111" s="23"/>
-      <c r="L111" s="23"/>
-      <c r="M111" s="23"/>
-      <c r="N111" s="23"/>
-      <c r="O111" s="22"/>
-      <c r="P111" s="26" t="s">
+      <c r="D111" s="22"/>
+      <c r="E111" s="22"/>
+      <c r="F111" s="22"/>
+      <c r="G111" s="22"/>
+      <c r="H111" s="22"/>
+      <c r="I111" s="22"/>
+      <c r="J111" s="22"/>
+      <c r="K111" s="22"/>
+      <c r="L111" s="22"/>
+      <c r="M111" s="22"/>
+      <c r="N111" s="22"/>
+      <c r="O111" s="21"/>
+      <c r="P111" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="Q111" s="26"/>
-      <c r="R111" s="26"/>
-      <c r="S111" s="26"/>
-      <c r="T111" s="26"/>
-      <c r="U111" s="26"/>
-      <c r="V111" s="26"/>
-      <c r="W111" s="26"/>
-      <c r="X111" s="26"/>
-      <c r="Y111" s="26"/>
-      <c r="Z111" s="26"/>
-      <c r="AA111" s="26"/>
-      <c r="AB111" s="26"/>
-      <c r="AC111" s="26"/>
-      <c r="AD111" s="26"/>
-      <c r="AE111" s="26"/>
-      <c r="AF111" s="26"/>
+      <c r="Q111" s="24"/>
+      <c r="R111" s="24"/>
+      <c r="S111" s="24"/>
+      <c r="T111" s="24"/>
+      <c r="U111" s="24"/>
+      <c r="V111" s="24"/>
+      <c r="W111" s="24"/>
+      <c r="X111" s="24"/>
+      <c r="Y111" s="24"/>
+      <c r="Z111" s="24"/>
+      <c r="AA111" s="24"/>
+      <c r="AB111" s="24"/>
+      <c r="AC111" s="24"/>
+      <c r="AD111" s="24"/>
+      <c r="AE111" s="24"/>
+      <c r="AF111" s="24"/>
     </row>
     <row r="112" spans="4:32" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D112"/>

</xml_diff>